<commit_message>
Final Forgot Password and Contact Page
</commit_message>
<xml_diff>
--- a/Final report/Contact Page/Testing Spreadsheet v1.0 ContactPage.xlsx
+++ b/Final report/Contact Page/Testing Spreadsheet v1.0 ContactPage.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonnie\Documents\Software Development\CSC7056 Software Testing &amp; Verification\Group Project\Software-Testing-And-Verification\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonnie\Documents\Software Development\CSC7056 Software Testing &amp; Verification\Group Project\Software-Testing-And-Verification\Final report\Contact Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection workbookPassword="A6C2" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="105" windowWidth="16560" windowHeight="6345" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="105" windowWidth="16560" windowHeight="6345" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Reqs" sheetId="5" r:id="rId1"/>
@@ -205,7 +205,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="342">
   <si>
     <t xml:space="preserve">Req </t>
   </si>
@@ -439,9 +439,6 @@
   </si>
   <si>
     <t>N/A</t>
-  </si>
-  <si>
-    <t>J Leathem</t>
   </si>
   <si>
     <r>
@@ -519,27 +516,6 @@
     </r>
   </si>
   <si>
-    <t>Contact_Tconn_1</t>
-  </si>
-  <si>
-    <t>Contact_Tconn_2</t>
-  </si>
-  <si>
-    <t>Contact_Tconn_3</t>
-  </si>
-  <si>
-    <t>Contact_Tconn_4</t>
-  </si>
-  <si>
-    <t>Tcase_1</t>
-  </si>
-  <si>
-    <t>Contact_1</t>
-  </si>
-  <si>
-    <t>Contact_Tproc_1</t>
-  </si>
-  <si>
     <t>While on the contact page check if contact details are consistent with the contact details in the requirements document.</t>
   </si>
   <si>
@@ -575,9 +551,6 @@
     <t>To show that if an unregistered or not logged-in user clicks on the email addresses in the Contact page the user's email client does not open.</t>
   </si>
   <si>
-    <t>Tcase_2</t>
-  </si>
-  <si>
     <t>On the Contact page.        Click on the support@pizzait.com link.</t>
   </si>
   <si>
@@ -587,12 +560,6 @@
     <t>Logged-in user: jleathem03@qub.ac.uk</t>
   </si>
   <si>
-    <t>Tcase_3</t>
-  </si>
-  <si>
-    <t>Tcase_4</t>
-  </si>
-  <si>
     <t>Check if a logged-in user clicks on the Marketing link on the Contact page that the user's email client opens with a new email message addressed orders@pizzait.com</t>
   </si>
   <si>
@@ -605,15 +572,6 @@
     <t>On the Contact page.        Click on the general@pizzait.com link.</t>
   </si>
   <si>
-    <t>Contact_Tproc_2</t>
-  </si>
-  <si>
-    <t>Contact_Tproc_3</t>
-  </si>
-  <si>
-    <t>Contact_Tproc_4</t>
-  </si>
-  <si>
     <t>The user's email client opens with a new email addressed as support@pizzait.com</t>
   </si>
   <si>
@@ -632,30 +590,12 @@
     <t>The user's email client opens with a new email addressed as general@pizzait.com</t>
   </si>
   <si>
-    <t>Tcase_5</t>
-  </si>
-  <si>
     <t>Check if an unregistered or not logged-in user clicks on the Support link on the Contact page that no email client is opened.</t>
   </si>
   <si>
     <t>On the Contact page.      Click on the support@pizzait.com link.</t>
   </si>
   <si>
-    <t>Tcase_6</t>
-  </si>
-  <si>
-    <t>Tcase_7</t>
-  </si>
-  <si>
-    <t>Contact_Tproc_5</t>
-  </si>
-  <si>
-    <t>Contact_Tproc_6</t>
-  </si>
-  <si>
-    <t>Contact_Tproc_7</t>
-  </si>
-  <si>
     <t>While not logged in and on the Contact page click on the Support link.</t>
   </si>
   <si>
@@ -668,9 +608,6 @@
     <t>No email client should open.</t>
   </si>
   <si>
-    <t>Tcase_8</t>
-  </si>
-  <si>
     <t>Check spelling and grammar on page.</t>
   </si>
   <si>
@@ -680,150 +617,84 @@
     <t>Contact_TConn_4</t>
   </si>
   <si>
-    <t>Contact_Tproc_8</t>
-  </si>
-  <si>
     <t>Go to page check for spelling or grammar mistakes.</t>
   </si>
   <si>
     <t>No spelling or grammar mistakes.</t>
   </si>
   <si>
-    <t>Contact_2</t>
-  </si>
-  <si>
-    <t>Contact_3</t>
-  </si>
-  <si>
-    <t>Contact_4</t>
-  </si>
-  <si>
     <t>Email client opened an email addressed from personal email address rather than from the user email address.</t>
   </si>
   <si>
     <t>Email client opened an email addressed from personal email address.</t>
   </si>
   <si>
-    <t>Contact_5</t>
-  </si>
-  <si>
-    <t>Contact_6</t>
-  </si>
-  <si>
-    <t>Contact_7</t>
-  </si>
-  <si>
-    <t>Contact_Tconn_5</t>
-  </si>
-  <si>
     <t>To show that the company logo displays on the header of the Contact page</t>
   </si>
   <si>
     <t>4.1.1</t>
   </si>
   <si>
-    <t>Contact_Tconn_6</t>
-  </si>
-  <si>
     <t>To show that the copyright and correct version information displays at the footer of the Contact page.</t>
   </si>
   <si>
     <t>4.1.2</t>
   </si>
   <si>
-    <t>Contact_Tconn_7</t>
-  </si>
-  <si>
     <t>To show that the correct page title displays on the Contact page</t>
   </si>
   <si>
     <t>4.1.4</t>
   </si>
   <si>
-    <t>low</t>
-  </si>
-  <si>
-    <t>Contact_Tconn_8</t>
-  </si>
-  <si>
     <t>To show that the "Contact" page exists as part of the system.</t>
   </si>
   <si>
     <t>4.1.5</t>
   </si>
   <si>
-    <t>Contact_Tconn_9</t>
-  </si>
-  <si>
     <t>To show there is a common navigational area on the Contact page</t>
   </si>
   <si>
     <t>4.1.7</t>
   </si>
   <si>
-    <t>Contact_Tconn_10</t>
-  </si>
-  <si>
     <t>To show that when the Home link is selected within the Contact page, the user is directed to the Home page</t>
   </si>
   <si>
     <t>4.1.8</t>
   </si>
   <si>
-    <t>Contact_Tconn_11</t>
-  </si>
-  <si>
     <t>To show that when Order is selected as a logged in user on the Contact page, the user is directed to the Order page.</t>
   </si>
   <si>
-    <t>Contact_Tconn_12</t>
-  </si>
-  <si>
     <t>To show that when Order is selected as a non-logged in user on the Contact page, the user is prevented from accessing the Order page</t>
   </si>
   <si>
-    <t>Contact_Tconn_13</t>
-  </si>
-  <si>
     <t>To show that when the About link is selected within the Contact page, the user is directed to the About page.</t>
   </si>
   <si>
-    <t>Contact_Tconn_14</t>
-  </si>
-  <si>
     <t>To show that a non-logged in user can directly navigate to the "Register" and "Log in" pages from the "Contact" page</t>
   </si>
   <si>
     <t>4.1.9</t>
   </si>
   <si>
-    <t>Contact_Tconn_15</t>
-  </si>
-  <si>
     <t>To show that a logged in user can directly navigate to the "My Account - reset password" page from the "Contact" page</t>
   </si>
   <si>
     <t>4.1.10</t>
   </si>
   <si>
-    <t>Contact_Tconn_16</t>
-  </si>
-  <si>
     <t>To show that a logged in user can log off from the "Contact" page</t>
   </si>
   <si>
-    <t>Contact_Tconn_17</t>
-  </si>
-  <si>
     <t>To show that the "Forgot password" page is not directly accessible from the "Contact" page</t>
   </si>
   <si>
     <t>4.1.11</t>
   </si>
   <si>
-    <t>Tcase_9</t>
-  </si>
-  <si>
     <t>Check if the logo displays upon the Contact page's header</t>
   </si>
   <si>
@@ -833,39 +704,21 @@
     <t>Kevin O'Hare</t>
   </si>
   <si>
-    <t>Tcase_10</t>
-  </si>
-  <si>
     <t>Check if the correct version information and copyright displays upon the Contact page's footer</t>
   </si>
   <si>
-    <t>Tcase_11</t>
-  </si>
-  <si>
     <t>Check if the Contact page has Contact as a title</t>
   </si>
   <si>
-    <t>Tcase_12</t>
-  </si>
-  <si>
     <t>Check if the Contact page exists as part of the website</t>
   </si>
   <si>
-    <t>Tcase_13</t>
-  </si>
-  <si>
     <t>Check if the Contact page has a common navigational area</t>
   </si>
   <si>
-    <t>Tcase_14</t>
-  </si>
-  <si>
     <t>Check if the Home page can be navigated to from the Contact page</t>
   </si>
   <si>
-    <t>Tcase_15</t>
-  </si>
-  <si>
     <t>Check if the Order page can be navigated to from the Contact page as a logged in user</t>
   </si>
   <si>
@@ -875,54 +728,30 @@
     <t>Username: kohare08@qub.ac.uk, password: simpson</t>
   </si>
   <si>
-    <t>Tcase_16</t>
-  </si>
-  <si>
     <t>Check if a non-logged in user is unable to navigate to Order from Contact</t>
   </si>
   <si>
     <t>On the Contact page as an unregistered user</t>
   </si>
   <si>
-    <t>Tcase_17</t>
-  </si>
-  <si>
     <t>Check if the About page can be navigated to from the Contact page</t>
   </si>
   <si>
-    <t>Tcase_18</t>
-  </si>
-  <si>
     <t>Check if the Register page can be directly navigated to from the Contact page as a non-logged in user</t>
   </si>
   <si>
-    <t>Tcase_19</t>
-  </si>
-  <si>
     <t>Check if the Log in page can be directly navigated to from the Contact page as a non-logged in user</t>
   </si>
   <si>
-    <t>Tcase_20</t>
-  </si>
-  <si>
     <t>Check if the My Account - reset password page can be directly navigated to from the Contact page as a logged in user</t>
   </si>
   <si>
-    <t>Tcase_21</t>
-  </si>
-  <si>
     <t>Check if a logged in user can log off from the "Contact" page</t>
   </si>
   <si>
-    <t>Tcase_22</t>
-  </si>
-  <si>
     <t>Check if the "Contact" page does not allow direct access to the "Forgot password" page</t>
   </si>
   <si>
-    <t>Contact_Tproc_9</t>
-  </si>
-  <si>
     <t>While on the Contact page check if the company logo displays properly within the header</t>
   </si>
   <si>
@@ -932,9 +761,6 @@
     <t>Displayed but a copyright watermark is visible</t>
   </si>
   <si>
-    <t>Contact_Tproc_10</t>
-  </si>
-  <si>
     <t>While on the Contact page check if the correct version infromation and copyright displays properly within the footer</t>
   </si>
   <si>
@@ -944,9 +770,6 @@
     <t>© 2015 - QUB CSC3056 CSC7056 Testing Site V1.0</t>
   </si>
   <si>
-    <t>Contact_Tproc_11</t>
-  </si>
-  <si>
     <t>While on the Contact page check if the title is 'Contact'</t>
   </si>
   <si>
@@ -956,90 +779,60 @@
     <t>Fine</t>
   </si>
   <si>
-    <t>Contact_Tproc_12</t>
-  </si>
-  <si>
     <t>While on the website system, check if the Contact page exists</t>
   </si>
   <si>
     <t>Contact page is accessible and displays when selected</t>
   </si>
   <si>
-    <t>Contact_Tproc_13</t>
-  </si>
-  <si>
     <t>While on the Contact page check if the page has a common navigational area</t>
   </si>
   <si>
     <t>Contact page will have a common navigational area</t>
   </si>
   <si>
-    <t>Contact_Tproc_14</t>
-  </si>
-  <si>
     <t>While on the Contact page select the Home link</t>
   </si>
   <si>
     <t>User is directed to the Home page</t>
   </si>
   <si>
-    <t>Contact_Tproc_15</t>
-  </si>
-  <si>
     <t>Log in using a valid username and password, direct to the Contact page and then direct to the Order page.</t>
   </si>
   <si>
     <t>User is allowed access to Order page</t>
   </si>
   <si>
-    <t>Contact_Tproc_16</t>
-  </si>
-  <si>
     <t>While on the Contact page as a non-logged in user select the Order link.</t>
   </si>
   <si>
     <t>User is prevented access to the Order page</t>
   </si>
   <si>
-    <t>Contact_Tproc_17</t>
-  </si>
-  <si>
     <t>While on the Contact page select the About link</t>
   </si>
   <si>
     <t>User is directed to the About page</t>
   </si>
   <si>
-    <t>Contact_Tproc_18</t>
-  </si>
-  <si>
     <t>While on the Contact page and not logged in, select the Register link</t>
   </si>
   <si>
     <t>User is directed to the Register page</t>
   </si>
   <si>
-    <t>Contact_Tproc_19</t>
-  </si>
-  <si>
     <t>While on the Contact page and not logged in, select the select the Log in link</t>
   </si>
   <si>
     <t>User is directed to the Log in page</t>
   </si>
   <si>
-    <t>Contact_Tproc_20</t>
-  </si>
-  <si>
     <t>While on the Contact page as a logged in user, select the My Account - reset password link</t>
   </si>
   <si>
     <t>User is directed to the My Account - reset password  page</t>
   </si>
   <si>
-    <t>Contact_Tproc_21</t>
-  </si>
-  <si>
     <t>While on the Contact page as a logged in user, select the Log off link</t>
   </si>
   <si>
@@ -1049,9 +842,6 @@
     <t>Fine, returned to Home page</t>
   </si>
   <si>
-    <t>Contact_Tproc_22</t>
-  </si>
-  <si>
     <t>While on the Contact page check if the Forgot password page is directly accessible</t>
   </si>
   <si>
@@ -1103,42 +893,6 @@
     <t>To show that logged in user can log off  from Contact page.</t>
   </si>
   <si>
-    <t>Contact_Tconn_18</t>
-  </si>
-  <si>
-    <t>Contact_Tconn_19</t>
-  </si>
-  <si>
-    <t>Contact_Tconn_20</t>
-  </si>
-  <si>
-    <t>Contact_Tconn_21</t>
-  </si>
-  <si>
-    <t>Contact_Tconn_22</t>
-  </si>
-  <si>
-    <t>Contact_Tconn_23</t>
-  </si>
-  <si>
-    <t>Contact_Tconn_24</t>
-  </si>
-  <si>
-    <t>Contact_Tconn_25</t>
-  </si>
-  <si>
-    <t>Contact_Tconn_26</t>
-  </si>
-  <si>
-    <t>Contact_Tconn_27</t>
-  </si>
-  <si>
-    <t>Contact_Tconn_28</t>
-  </si>
-  <si>
-    <t>Contact_Tconn_29</t>
-  </si>
-  <si>
     <t>Check that unregistered users or registered but not logged in users cannot access the Ordering Pizza page, Schedule page, Receipt page or My Account - reset password page from the Contact page.</t>
   </si>
   <si>
@@ -1205,57 +959,6 @@
     <t>Check that logged in user can log off  from Contact page.</t>
   </si>
   <si>
-    <t>Tcase_23</t>
-  </si>
-  <si>
-    <t>Tcase_24</t>
-  </si>
-  <si>
-    <t>Tcase_25</t>
-  </si>
-  <si>
-    <t>Tcase_26</t>
-  </si>
-  <si>
-    <t>Tcase_27</t>
-  </si>
-  <si>
-    <t>Tcase_28</t>
-  </si>
-  <si>
-    <t>Tcase_29</t>
-  </si>
-  <si>
-    <t>Tcase_30</t>
-  </si>
-  <si>
-    <t>Tcase_31</t>
-  </si>
-  <si>
-    <t>Tcase_32</t>
-  </si>
-  <si>
-    <t>Tcase_33</t>
-  </si>
-  <si>
-    <t>Tcase_34</t>
-  </si>
-  <si>
-    <t>Tcase_35</t>
-  </si>
-  <si>
-    <t>Tcase_36</t>
-  </si>
-  <si>
-    <t>Contact_8</t>
-  </si>
-  <si>
-    <t>Contact_10</t>
-  </si>
-  <si>
-    <t>Contact_11</t>
-  </si>
-  <si>
     <t xml:space="preserve">Do not log in to the website. While on the Contact page and not logged in, click on the "Order" button on the navigation to make sure user is directed to login page. Click on "Contact" on navigation to return to Contact page. Enter the URL for the Ordering Pizza page (http://lamp.eeecs.qub.ac.uk:8080/Members/OrderPizza.aspx) and click enter and confirm user arrives on login page.   Click on "Contact" on navigation to return to Contact page. Enter the URL for the Schedule page (http://lamp.eeecs.qub.ac.uk:8080/Members/Order.aspx) and click enter and confirm user arrives on login page.  Click on "Contact" on navigation to return to Contact page. Enter the URL for the Receipt page (http://lamp.eeecs.qub.ac.uk:8080/Members/OrderReceipt.aspx) and click enter and confirm user arrives on login page.  Click on "Contact" on navigation to return to Contact page.   Enter the URL for the My Account - reset password  page (http://lamp.eeecs.qub.ac.uk:8080/Members/Manage) and click enter and confirm user arrives on login page.  </t>
   </si>
   <si>
@@ -1325,49 +1028,340 @@
     <t>The top right corner where the log off button was should now have "Register" and "Login" in its stead. User should end up on the Login page, evidencing being logged out, when "Order" is clicked.</t>
   </si>
   <si>
-    <t>Contact_Tproc_23</t>
-  </si>
-  <si>
-    <t>Contact_Tproc_24</t>
-  </si>
-  <si>
-    <t>Contact_Tproc_25</t>
-  </si>
-  <si>
-    <t>Contact_Tproc_26</t>
-  </si>
-  <si>
-    <t>Contact_Tproc_27</t>
-  </si>
-  <si>
-    <t>Contact_Tproc_28</t>
-  </si>
-  <si>
-    <t>Contact_Tproc_29</t>
-  </si>
-  <si>
-    <t>Contact_Tproc_30</t>
-  </si>
-  <si>
-    <t>Contact_Tproc_31</t>
-  </si>
-  <si>
-    <t>Contact_Tproc_32</t>
-  </si>
-  <si>
-    <t>Contact_Tproc_33</t>
-  </si>
-  <si>
-    <t>Contact_Tproc_34</t>
-  </si>
-  <si>
-    <t>Contact_Tproc_35</t>
-  </si>
-  <si>
-    <t>Contact_Tproc_36</t>
-  </si>
-  <si>
-    <t>J Leathem &amp; Jack Ferguson</t>
+    <t>Contact_TConn_1</t>
+  </si>
+  <si>
+    <t>Contact_TConn_2</t>
+  </si>
+  <si>
+    <t>Contact_TConn_3</t>
+  </si>
+  <si>
+    <t>Contact_TConn_5</t>
+  </si>
+  <si>
+    <t>Contact_TConn_6</t>
+  </si>
+  <si>
+    <t>Contact_TConn_7</t>
+  </si>
+  <si>
+    <t>Contact_TConn_8</t>
+  </si>
+  <si>
+    <t>Contact_TConn_9</t>
+  </si>
+  <si>
+    <t>Contact_TConn_10</t>
+  </si>
+  <si>
+    <t>Contact_TConn_11</t>
+  </si>
+  <si>
+    <t>Contact_TConn_12</t>
+  </si>
+  <si>
+    <t>Contact_TConn_13</t>
+  </si>
+  <si>
+    <t>Contact_TConn_14</t>
+  </si>
+  <si>
+    <t>Contact_TConn_15</t>
+  </si>
+  <si>
+    <t>Contact_TConn_16</t>
+  </si>
+  <si>
+    <t>Contact_TConn_17</t>
+  </si>
+  <si>
+    <t>Contact_TConn_18</t>
+  </si>
+  <si>
+    <t>Contact_TConn_19</t>
+  </si>
+  <si>
+    <t>Contact_TConn_20</t>
+  </si>
+  <si>
+    <t>Contact_TConn_21</t>
+  </si>
+  <si>
+    <t>Contact_TConn_22</t>
+  </si>
+  <si>
+    <t>Contact_TConn_23</t>
+  </si>
+  <si>
+    <t>Contact_TConn_24</t>
+  </si>
+  <si>
+    <t>Contact_TConn_25</t>
+  </si>
+  <si>
+    <t>Contact_TConn_26</t>
+  </si>
+  <si>
+    <t>Contact_TConn_27</t>
+  </si>
+  <si>
+    <t>Contact_TConn_28</t>
+  </si>
+  <si>
+    <t>Contact_TConn_29</t>
+  </si>
+  <si>
+    <t>TCase_1</t>
+  </si>
+  <si>
+    <t>TCase_2</t>
+  </si>
+  <si>
+    <t>TCase_3</t>
+  </si>
+  <si>
+    <t>TCase_4</t>
+  </si>
+  <si>
+    <t>TCase_5</t>
+  </si>
+  <si>
+    <t>TCase_6</t>
+  </si>
+  <si>
+    <t>TCase_7</t>
+  </si>
+  <si>
+    <t>TCase_8</t>
+  </si>
+  <si>
+    <t>TCase_9</t>
+  </si>
+  <si>
+    <t>TCase_10</t>
+  </si>
+  <si>
+    <t>TCase_11</t>
+  </si>
+  <si>
+    <t>TCase_12</t>
+  </si>
+  <si>
+    <t>TCase_13</t>
+  </si>
+  <si>
+    <t>TCase_14</t>
+  </si>
+  <si>
+    <t>TCase_15</t>
+  </si>
+  <si>
+    <t>TCase_16</t>
+  </si>
+  <si>
+    <t>TCase_17</t>
+  </si>
+  <si>
+    <t>TCase_18</t>
+  </si>
+  <si>
+    <t>TCase_19</t>
+  </si>
+  <si>
+    <t>TCase_20</t>
+  </si>
+  <si>
+    <t>TCase_21</t>
+  </si>
+  <si>
+    <t>TCase_22</t>
+  </si>
+  <si>
+    <t>TCase_23</t>
+  </si>
+  <si>
+    <t>TCase_24</t>
+  </si>
+  <si>
+    <t>TCase_25</t>
+  </si>
+  <si>
+    <t>TCase_26</t>
+  </si>
+  <si>
+    <t>TCase_27</t>
+  </si>
+  <si>
+    <t>TCase_28</t>
+  </si>
+  <si>
+    <t>TCase_29</t>
+  </si>
+  <si>
+    <t>TCase_30</t>
+  </si>
+  <si>
+    <t>TCase_31</t>
+  </si>
+  <si>
+    <t>TCase_32</t>
+  </si>
+  <si>
+    <t>TCase_33</t>
+  </si>
+  <si>
+    <t>TCase_34</t>
+  </si>
+  <si>
+    <t>TCase_35</t>
+  </si>
+  <si>
+    <t>TCase_36</t>
+  </si>
+  <si>
+    <t>Contact_Defect_1</t>
+  </si>
+  <si>
+    <t>Contact_Defect_2</t>
+  </si>
+  <si>
+    <t>Contact_Defect_3</t>
+  </si>
+  <si>
+    <t>Contact_Defect_4</t>
+  </si>
+  <si>
+    <t>Contact_Defect_5</t>
+  </si>
+  <si>
+    <t>Contact_Defect_6</t>
+  </si>
+  <si>
+    <t>Contact_Defect_7</t>
+  </si>
+  <si>
+    <t>Contact_Defect_8</t>
+  </si>
+  <si>
+    <t>Contact_Defect_10</t>
+  </si>
+  <si>
+    <t>Contact_Defect_11</t>
+  </si>
+  <si>
+    <t>Jonathan Leathem</t>
+  </si>
+  <si>
+    <t>Jonathan Leathem &amp; Jack Ferguson</t>
+  </si>
+  <si>
+    <t>Contact_TProc_1</t>
+  </si>
+  <si>
+    <t>Contact_TProc_2</t>
+  </si>
+  <si>
+    <t>Contact_TProc_3</t>
+  </si>
+  <si>
+    <t>Contact_TProc_4</t>
+  </si>
+  <si>
+    <t>Contact_TProc_5</t>
+  </si>
+  <si>
+    <t>Contact_TProc_6</t>
+  </si>
+  <si>
+    <t>Contact_TProc_7</t>
+  </si>
+  <si>
+    <t>Contact_TProc_8</t>
+  </si>
+  <si>
+    <t>Contact_TProc_9</t>
+  </si>
+  <si>
+    <t>Contact_TProc_10</t>
+  </si>
+  <si>
+    <t>Contact_TProc_11</t>
+  </si>
+  <si>
+    <t>Contact_TProc_12</t>
+  </si>
+  <si>
+    <t>Contact_TProc_13</t>
+  </si>
+  <si>
+    <t>Contact_TProc_14</t>
+  </si>
+  <si>
+    <t>Contact_TProc_15</t>
+  </si>
+  <si>
+    <t>Contact_TProc_16</t>
+  </si>
+  <si>
+    <t>Contact_TProc_17</t>
+  </si>
+  <si>
+    <t>Contact_TProc_18</t>
+  </si>
+  <si>
+    <t>Contact_TProc_19</t>
+  </si>
+  <si>
+    <t>Contact_TProc_20</t>
+  </si>
+  <si>
+    <t>Contact_TProc_21</t>
+  </si>
+  <si>
+    <t>Contact_TProc_22</t>
+  </si>
+  <si>
+    <t>Contact_TProc_23</t>
+  </si>
+  <si>
+    <t>Contact_TProc_24</t>
+  </si>
+  <si>
+    <t>Contact_TProc_25</t>
+  </si>
+  <si>
+    <t>Contact_TProc_26</t>
+  </si>
+  <si>
+    <t>Contact_TProc_27</t>
+  </si>
+  <si>
+    <t>Contact_TProc_28</t>
+  </si>
+  <si>
+    <t>Contact_TProc_29</t>
+  </si>
+  <si>
+    <t>Contact_TProc_30</t>
+  </si>
+  <si>
+    <t>Contact_TProc_31</t>
+  </si>
+  <si>
+    <t>Contact_TProc_32</t>
+  </si>
+  <si>
+    <t>Contact_TProc_33</t>
+  </si>
+  <si>
+    <t>Contact_TProc_34</t>
+  </si>
+  <si>
+    <t>Contact_TProc_35</t>
+  </si>
+  <si>
+    <t>Contact_TProc_36</t>
   </si>
 </sst>
 </file>
@@ -1941,11 +1935,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="1393377264"/>
-        <c:axId val="1393371280"/>
+        <c:axId val="-965963952"/>
+        <c:axId val="-965960688"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1393377264"/>
+        <c:axId val="-965963952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1955,7 +1949,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1393371280"/>
+        <c:crossAx val="-965960688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1963,7 +1957,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1393371280"/>
+        <c:axId val="-965960688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1974,7 +1968,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1393377264"/>
+        <c:crossAx val="-965963952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2445,8 +2439,8 @@
   </sheetPr>
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView topLeftCell="A9" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2472,7 +2466,7 @@
     </row>
     <row r="2" spans="1:9" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>68</v>
+        <v>230</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>59</v>
@@ -2489,10 +2483,10 @@
     </row>
     <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>60</v>
@@ -2504,10 +2498,10 @@
     </row>
     <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>78</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>60</v>
@@ -2519,7 +2513,7 @@
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>61</v>
@@ -2536,13 +2530,13 @@
     </row>
     <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>125</v>
+        <v>233</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>126</v>
+        <v>97</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>127</v>
+        <v>98</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -2553,13 +2547,13 @@
     </row>
     <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>128</v>
+        <v>234</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>129</v>
+        <v>99</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -2570,16 +2564,16 @@
     </row>
     <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>131</v>
+        <v>235</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>132</v>
+        <v>101</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>133</v>
+        <v>102</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>134</v>
+        <v>11</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>45</v>
@@ -2587,13 +2581,13 @@
     </row>
     <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>135</v>
+        <v>236</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>136</v>
+        <v>103</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>137</v>
+        <v>104</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>6</v>
@@ -2604,13 +2598,13 @@
     </row>
     <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>138</v>
+        <v>237</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>139</v>
+        <v>105</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>140</v>
+        <v>106</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>27</v>
@@ -2618,13 +2612,13 @@
     </row>
     <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>141</v>
+        <v>238</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>142</v>
+        <v>107</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>143</v>
+        <v>108</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>6</v>
@@ -2632,13 +2626,13 @@
     </row>
     <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>144</v>
+        <v>239</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>145</v>
+        <v>109</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>143</v>
+        <v>108</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>6</v>
@@ -2646,13 +2640,13 @@
     </row>
     <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>146</v>
+        <v>240</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>147</v>
+        <v>110</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>143</v>
+        <v>108</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>6</v>
@@ -2660,13 +2654,13 @@
     </row>
     <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>148</v>
+        <v>241</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>149</v>
+        <v>111</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>143</v>
+        <v>108</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>6</v>
@@ -2674,13 +2668,13 @@
     </row>
     <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>150</v>
+        <v>242</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>151</v>
+        <v>112</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>152</v>
+        <v>113</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>6</v>
@@ -2688,13 +2682,13 @@
     </row>
     <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>153</v>
+        <v>243</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>154</v>
+        <v>114</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>155</v>
+        <v>115</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>6</v>
@@ -2702,13 +2696,13 @@
     </row>
     <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>156</v>
+        <v>244</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>157</v>
+        <v>116</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>155</v>
+        <v>115</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>6</v>
@@ -2716,27 +2710,27 @@
     </row>
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>158</v>
+        <v>245</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>159</v>
+        <v>117</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>160</v>
+        <v>118</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="B19" s="34" t="s">
-        <v>241</v>
+        <v>171</v>
       </c>
       <c r="C19" s="34" t="s">
-        <v>242</v>
+        <v>172</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>6</v>
@@ -2744,13 +2738,13 @@
     </row>
     <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="B20" s="34" t="s">
-        <v>243</v>
+        <v>173</v>
       </c>
       <c r="C20" s="34" t="s">
-        <v>244</v>
+        <v>174</v>
       </c>
       <c r="D20" s="34" t="s">
         <v>6</v>
@@ -2758,13 +2752,13 @@
     </row>
     <row r="21" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="B21" s="34" t="s">
-        <v>245</v>
+        <v>175</v>
       </c>
       <c r="C21" s="34" t="s">
-        <v>244</v>
+        <v>174</v>
       </c>
       <c r="D21" s="34" t="s">
         <v>6</v>
@@ -2772,10 +2766,10 @@
     </row>
     <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>246</v>
+        <v>176</v>
       </c>
       <c r="C22" s="34" t="s">
         <v>62</v>
@@ -2786,10 +2780,10 @@
     </row>
     <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="B23" s="34" t="s">
-        <v>247</v>
+        <v>177</v>
       </c>
       <c r="C23" s="34" t="s">
         <v>62</v>
@@ -2800,10 +2794,10 @@
     </row>
     <row r="24" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="B24" s="34" t="s">
-        <v>248</v>
+        <v>178</v>
       </c>
       <c r="C24" s="34" t="s">
         <v>62</v>
@@ -2814,10 +2808,10 @@
     </row>
     <row r="25" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="B25" s="34" t="s">
-        <v>249</v>
+        <v>179</v>
       </c>
       <c r="C25" s="34" t="s">
         <v>62</v>
@@ -2828,10 +2822,10 @@
     </row>
     <row r="26" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="B26" s="34" t="s">
-        <v>250</v>
+        <v>180</v>
       </c>
       <c r="C26" s="34" t="s">
         <v>62</v>
@@ -2842,10 +2836,10 @@
     </row>
     <row r="27" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="B27" s="34" t="s">
-        <v>251</v>
+        <v>181</v>
       </c>
       <c r="C27" s="34" t="s">
         <v>62</v>
@@ -2856,10 +2850,10 @@
     </row>
     <row r="28" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="B28" s="34" t="s">
-        <v>252</v>
+        <v>182</v>
       </c>
       <c r="C28" s="34" t="s">
         <v>62</v>
@@ -2870,10 +2864,10 @@
     </row>
     <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="B29" s="34" t="s">
-        <v>253</v>
+        <v>183</v>
       </c>
       <c r="C29" s="34" t="s">
         <v>62</v>
@@ -2884,10 +2878,10 @@
     </row>
     <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="B30" s="34" t="s">
-        <v>254</v>
+        <v>184</v>
       </c>
       <c r="C30" s="34" t="s">
         <v>62</v>
@@ -2940,8 +2934,8 @@
   </sheetPr>
   <dimension ref="A1:Z160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E6" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView topLeftCell="A33" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3013,7 +3007,7 @@
     </row>
     <row r="2" spans="1:26" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>72</v>
+        <v>258</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>64</v>
@@ -3025,7 +3019,7 @@
         <v>65</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>68</v>
+        <v>230</v>
       </c>
       <c r="F2" s="10" t="s">
         <v>6</v>
@@ -3037,10 +3031,10 @@
         <v>25</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>66</v>
+        <v>304</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>73</v>
+        <v>294</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>33</v>
@@ -3053,28 +3047,28 @@
       </c>
       <c r="N2" s="32"/>
       <c r="O2" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P2" s="9"/>
       <c r="S2" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="114" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>79</v>
+        <v>259</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>69</v>
+        <v>231</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>6</v>
@@ -3085,11 +3079,11 @@
       <c r="H3" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="35" t="s">
-        <v>66</v>
+      <c r="I3" s="11" t="s">
+        <v>304</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>117</v>
+        <v>295</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>33</v>
@@ -3102,7 +3096,7 @@
       </c>
       <c r="N3" s="32"/>
       <c r="O3" s="3" t="s">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="P3" s="9"/>
       <c r="T3" s="27" t="s">
@@ -3111,19 +3105,19 @@
     </row>
     <row r="4" spans="1:26" ht="114" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>83</v>
+        <v>260</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>69</v>
+        <v>231</v>
       </c>
       <c r="F4" s="10" t="s">
         <v>6</v>
@@ -3134,11 +3128,11 @@
       <c r="H4" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="35" t="s">
-        <v>66</v>
+      <c r="I4" s="11" t="s">
+        <v>304</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>118</v>
+        <v>296</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>33</v>
@@ -3151,7 +3145,7 @@
       </c>
       <c r="N4" s="32"/>
       <c r="O4" s="3" t="s">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="P4" s="9"/>
       <c r="Z4" s="5" t="s">
@@ -3160,19 +3154,19 @@
     </row>
     <row r="5" spans="1:26" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>84</v>
+        <v>261</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>69</v>
+        <v>231</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>6</v>
@@ -3183,11 +3177,11 @@
       <c r="H5" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="35" t="s">
-        <v>66</v>
+      <c r="I5" s="11" t="s">
+        <v>304</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>119</v>
+        <v>297</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>33</v>
@@ -3200,25 +3194,25 @@
       </c>
       <c r="N5" s="32"/>
       <c r="O5" s="3" t="s">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="P5" s="9"/>
     </row>
     <row r="6" spans="1:26" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>98</v>
+        <v>262</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>70</v>
+        <v>232</v>
       </c>
       <c r="F6" s="10" t="s">
         <v>27</v>
@@ -3229,11 +3223,11 @@
       <c r="H6" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="13" t="s">
-        <v>66</v>
+      <c r="I6" s="11" t="s">
+        <v>304</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>122</v>
+        <v>298</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>33</v>
@@ -3246,25 +3240,25 @@
       </c>
       <c r="N6" s="32"/>
       <c r="O6" s="3" t="s">
-        <v>121</v>
+        <v>96</v>
       </c>
       <c r="P6" s="9"/>
     </row>
     <row r="7" spans="1:26" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>101</v>
+        <v>263</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>70</v>
+        <v>232</v>
       </c>
       <c r="F7" s="10" t="s">
         <v>27</v>
@@ -3275,11 +3269,11 @@
       <c r="H7" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="13" t="s">
-        <v>66</v>
+      <c r="I7" s="11" t="s">
+        <v>304</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>123</v>
+        <v>299</v>
       </c>
       <c r="K7" s="4" t="s">
         <v>33</v>
@@ -3292,7 +3286,7 @@
       </c>
       <c r="N7" s="32"/>
       <c r="O7" s="3" t="s">
-        <v>121</v>
+        <v>96</v>
       </c>
       <c r="P7" s="9"/>
       <c r="T7" t="s">
@@ -3301,19 +3295,19 @@
     </row>
     <row r="8" spans="1:26" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>102</v>
+        <v>264</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>70</v>
+        <v>232</v>
       </c>
       <c r="F8" s="10" t="s">
         <v>27</v>
@@ -3324,11 +3318,11 @@
       <c r="H8" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="I8" s="13" t="s">
-        <v>66</v>
+      <c r="I8" s="11" t="s">
+        <v>304</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>124</v>
+        <v>300</v>
       </c>
       <c r="K8" s="4" t="s">
         <v>33</v>
@@ -3341,7 +3335,7 @@
       </c>
       <c r="N8" s="32"/>
       <c r="O8" s="3" t="s">
-        <v>121</v>
+        <v>96</v>
       </c>
       <c r="P8" s="9"/>
       <c r="T8" t="s">
@@ -3353,20 +3347,20 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>110</v>
+      <c r="A9" s="3" t="s">
+        <v>265</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>113</v>
+        <v>92</v>
       </c>
       <c r="F9" s="10" t="s">
         <v>27</v>
@@ -3378,7 +3372,7 @@
         <v>24</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>343</v>
+        <v>305</v>
       </c>
       <c r="J9" s="9"/>
       <c r="K9" s="4"/>
@@ -3397,19 +3391,19 @@
     </row>
     <row r="10" spans="1:26" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>161</v>
+        <v>266</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>162</v>
+        <v>119</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>63</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>163</v>
+        <v>120</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>125</v>
+        <v>233</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>11</v>
@@ -3421,7 +3415,7 @@
         <v>24</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>164</v>
+        <v>121</v>
       </c>
       <c r="J10" s="9"/>
       <c r="K10" s="4"/>
@@ -3440,19 +3434,19 @@
     </row>
     <row r="11" spans="1:26" ht="57" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>165</v>
+        <v>267</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>166</v>
+        <v>122</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>63</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>163</v>
+        <v>120</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>128</v>
+        <v>234</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>11</v>
@@ -3464,7 +3458,7 @@
         <v>24</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>164</v>
+        <v>121</v>
       </c>
       <c r="J11" s="9"/>
       <c r="K11" s="4"/>
@@ -3476,19 +3470,19 @@
     </row>
     <row r="12" spans="1:26" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>167</v>
+        <v>268</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>168</v>
+        <v>123</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>63</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>163</v>
+        <v>120</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>131</v>
+        <v>235</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>11</v>
@@ -3500,7 +3494,7 @@
         <v>24</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>164</v>
+        <v>121</v>
       </c>
       <c r="J12" s="9"/>
       <c r="K12" s="9"/>
@@ -3512,19 +3506,19 @@
     </row>
     <row r="13" spans="1:26" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>169</v>
+        <v>269</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>170</v>
+        <v>124</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>63</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>163</v>
+        <v>120</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>135</v>
+        <v>236</v>
       </c>
       <c r="F13" s="10" t="s">
         <v>6</v>
@@ -3536,7 +3530,7 @@
         <v>24</v>
       </c>
       <c r="I13" s="11" t="s">
-        <v>164</v>
+        <v>121</v>
       </c>
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
@@ -3548,19 +3542,19 @@
     </row>
     <row r="14" spans="1:26" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>171</v>
+        <v>270</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>172</v>
+        <v>125</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>63</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>163</v>
+        <v>120</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>138</v>
+        <v>237</v>
       </c>
       <c r="F14" s="10" t="s">
         <v>27</v>
@@ -3572,7 +3566,7 @@
         <v>24</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>164</v>
+        <v>121</v>
       </c>
       <c r="J14" s="9"/>
       <c r="K14" s="9"/>
@@ -3584,19 +3578,19 @@
     </row>
     <row r="15" spans="1:26" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>173</v>
+        <v>271</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>174</v>
+        <v>126</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>63</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>163</v>
+        <v>120</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>141</v>
+        <v>238</v>
       </c>
       <c r="F15" s="10" t="s">
         <v>6</v>
@@ -3608,7 +3602,7 @@
         <v>24</v>
       </c>
       <c r="I15" s="11" t="s">
-        <v>164</v>
+        <v>121</v>
       </c>
       <c r="J15" s="9"/>
       <c r="K15" s="9"/>
@@ -3620,19 +3614,19 @@
     </row>
     <row r="16" spans="1:26" ht="57" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>175</v>
+        <v>272</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>176</v>
+        <v>127</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>177</v>
+        <v>128</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>178</v>
+        <v>129</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>144</v>
+        <v>239</v>
       </c>
       <c r="F16" s="10" t="s">
         <v>6</v>
@@ -3644,7 +3638,7 @@
         <v>24</v>
       </c>
       <c r="I16" s="11" t="s">
-        <v>164</v>
+        <v>121</v>
       </c>
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
@@ -3656,19 +3650,19 @@
     </row>
     <row r="17" spans="1:21" ht="57" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>179</v>
+        <v>273</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>180</v>
+        <v>130</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>181</v>
+        <v>131</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>163</v>
+        <v>120</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>146</v>
+        <v>240</v>
       </c>
       <c r="F17" s="10" t="s">
         <v>6</v>
@@ -3680,7 +3674,7 @@
         <v>24</v>
       </c>
       <c r="I17" s="11" t="s">
-        <v>164</v>
+        <v>121</v>
       </c>
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
@@ -3692,19 +3686,19 @@
     </row>
     <row r="18" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>182</v>
+        <v>274</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>183</v>
+        <v>132</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>63</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>163</v>
+        <v>120</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>148</v>
+        <v>241</v>
       </c>
       <c r="F18" s="10" t="s">
         <v>6</v>
@@ -3716,7 +3710,7 @@
         <v>24</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>164</v>
+        <v>121</v>
       </c>
       <c r="J18" s="9"/>
       <c r="K18" s="9"/>
@@ -3728,19 +3722,19 @@
     </row>
     <row r="19" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>184</v>
+        <v>275</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>185</v>
+        <v>133</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>63</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>163</v>
+        <v>120</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>150</v>
+        <v>242</v>
       </c>
       <c r="F19" s="10" t="s">
         <v>6</v>
@@ -3752,7 +3746,7 @@
         <v>24</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>164</v>
+        <v>121</v>
       </c>
       <c r="J19" s="9"/>
       <c r="K19" s="9"/>
@@ -3764,19 +3758,19 @@
     </row>
     <row r="20" spans="1:21" ht="57" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>186</v>
+        <v>276</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>187</v>
+        <v>134</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>63</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>163</v>
+        <v>120</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>150</v>
+        <v>242</v>
       </c>
       <c r="F20" s="10" t="s">
         <v>6</v>
@@ -3788,7 +3782,7 @@
         <v>24</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>164</v>
+        <v>121</v>
       </c>
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
@@ -3800,19 +3794,19 @@
     </row>
     <row r="21" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>188</v>
+        <v>277</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>189</v>
+        <v>135</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>177</v>
+        <v>128</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>178</v>
+        <v>129</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>153</v>
+        <v>243</v>
       </c>
       <c r="F21" s="10" t="s">
         <v>6</v>
@@ -3824,7 +3818,7 @@
         <v>24</v>
       </c>
       <c r="I21" s="11" t="s">
-        <v>164</v>
+        <v>121</v>
       </c>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
@@ -3836,19 +3830,19 @@
     </row>
     <row r="22" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>190</v>
+        <v>278</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>191</v>
+        <v>136</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>177</v>
+        <v>128</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>178</v>
+        <v>129</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>156</v>
+        <v>244</v>
       </c>
       <c r="F22" s="10" t="s">
         <v>6</v>
@@ -3860,7 +3854,7 @@
         <v>24</v>
       </c>
       <c r="I22" s="11" t="s">
-        <v>164</v>
+        <v>121</v>
       </c>
       <c r="J22" s="9"/>
       <c r="K22" s="9"/>
@@ -3872,22 +3866,22 @@
     </row>
     <row r="23" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>192</v>
+        <v>279</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>193</v>
+        <v>137</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>63</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>163</v>
+        <v>120</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>11</v>
+        <v>245</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>6</v>
       </c>
       <c r="G23" s="12">
         <v>42108</v>
@@ -3896,7 +3890,7 @@
         <v>24</v>
       </c>
       <c r="I23" s="11" t="s">
-        <v>164</v>
+        <v>121</v>
       </c>
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
@@ -3908,19 +3902,19 @@
     </row>
     <row r="24" spans="1:21" ht="128.25" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>267</v>
+        <v>185</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>268</v>
+        <v>186</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="F24" s="10" t="s">
         <v>6</v>
@@ -3932,7 +3926,7 @@
         <v>24</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>269</v>
+        <v>187</v>
       </c>
       <c r="J24" s="3"/>
       <c r="K24" s="4"/>
@@ -3944,19 +3938,19 @@
     </row>
     <row r="25" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>270</v>
+        <v>188</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>271</v>
+        <v>189</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="F25" s="10" t="s">
         <v>6</v>
@@ -3968,7 +3962,7 @@
         <v>24</v>
       </c>
       <c r="I25" s="13" t="s">
-        <v>269</v>
+        <v>187</v>
       </c>
       <c r="J25" s="35"/>
       <c r="K25" s="4"/>
@@ -3981,21 +3975,21 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" ht="114" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>272</v>
+        <v>190</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>273</v>
+        <v>191</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>274</v>
+        <v>192</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="F26" s="10" t="s">
         <v>6</v>
@@ -4007,7 +4001,7 @@
         <v>24</v>
       </c>
       <c r="I26" s="13" t="s">
-        <v>269</v>
+        <v>187</v>
       </c>
       <c r="J26" s="35"/>
       <c r="K26" s="4"/>
@@ -4026,19 +4020,19 @@
     </row>
     <row r="27" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>275</v>
+        <v>193</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>271</v>
+        <v>189</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="F27" s="10" t="s">
         <v>6</v>
@@ -4050,7 +4044,7 @@
         <v>24</v>
       </c>
       <c r="I27" s="13" t="s">
-        <v>269</v>
+        <v>187</v>
       </c>
       <c r="J27" s="35"/>
       <c r="K27" s="4"/>
@@ -4069,19 +4063,19 @@
     </row>
     <row r="28" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>275</v>
+        <v>193</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>273</v>
+        <v>191</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>274</v>
+        <v>192</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="F28" s="10" t="s">
         <v>6</v>
@@ -4093,7 +4087,7 @@
         <v>24</v>
       </c>
       <c r="I28" s="13" t="s">
-        <v>269</v>
+        <v>187</v>
       </c>
       <c r="J28" s="9"/>
       <c r="K28" s="4"/>
@@ -4112,19 +4106,19 @@
     </row>
     <row r="29" spans="1:21" ht="135" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>276</v>
+        <v>194</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>277</v>
+        <v>195</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>258</v>
+      <c r="E29" s="11" t="s">
+        <v>249</v>
       </c>
       <c r="F29" s="10" t="s">
         <v>11</v>
@@ -4136,10 +4130,10 @@
         <v>25</v>
       </c>
       <c r="I29" s="9" t="s">
-        <v>269</v>
+        <v>187</v>
       </c>
       <c r="J29" s="9" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="K29" s="4" t="s">
         <v>33</v>
@@ -4152,7 +4146,7 @@
       </c>
       <c r="N29" s="9"/>
       <c r="O29" s="1" t="s">
-        <v>278</v>
+        <v>196</v>
       </c>
       <c r="P29" s="9"/>
       <c r="T29" t="s">
@@ -4165,19 +4159,19 @@
     </row>
     <row r="30" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>279</v>
+        <v>197</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>277</v>
+        <v>195</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E30" s="1" t="s">
-        <v>259</v>
+      <c r="E30" s="11" t="s">
+        <v>250</v>
       </c>
       <c r="F30" s="10" t="s">
         <v>11</v>
@@ -4189,7 +4183,7 @@
         <v>24</v>
       </c>
       <c r="I30" s="9" t="s">
-        <v>269</v>
+        <v>187</v>
       </c>
       <c r="J30" s="9"/>
       <c r="K30" s="4"/>
@@ -4208,19 +4202,19 @@
     </row>
     <row r="31" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>280</v>
+        <v>198</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>277</v>
+        <v>195</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>260</v>
+      <c r="E31" s="11" t="s">
+        <v>251</v>
       </c>
       <c r="F31" s="10" t="s">
         <v>27</v>
@@ -4232,7 +4226,7 @@
         <v>24</v>
       </c>
       <c r="I31" s="9" t="s">
-        <v>269</v>
+        <v>187</v>
       </c>
       <c r="J31" s="9"/>
       <c r="K31" s="4"/>
@@ -4244,19 +4238,19 @@
     </row>
     <row r="32" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>281</v>
+        <v>199</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>277</v>
+        <v>195</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E32" s="1" t="s">
-        <v>261</v>
+      <c r="E32" s="11" t="s">
+        <v>252</v>
       </c>
       <c r="F32" s="10" t="s">
         <v>27</v>
@@ -4268,7 +4262,7 @@
         <v>24</v>
       </c>
       <c r="I32" s="9" t="s">
-        <v>269</v>
+        <v>187</v>
       </c>
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
@@ -4280,19 +4274,19 @@
     </row>
     <row r="33" spans="1:16" ht="120" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>282</v>
+        <v>200</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>277</v>
+        <v>195</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E33" s="1" t="s">
-        <v>262</v>
+      <c r="E33" s="11" t="s">
+        <v>253</v>
       </c>
       <c r="F33" s="10" t="s">
         <v>27</v>
@@ -4304,10 +4298,10 @@
         <v>25</v>
       </c>
       <c r="I33" s="9" t="s">
-        <v>269</v>
+        <v>187</v>
       </c>
       <c r="J33" s="9" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="K33" s="4" t="s">
         <v>33</v>
@@ -4320,25 +4314,25 @@
       </c>
       <c r="N33" s="9"/>
       <c r="O33" s="1" t="s">
-        <v>283</v>
+        <v>201</v>
       </c>
       <c r="P33" s="9"/>
     </row>
     <row r="34" spans="1:16" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>284</v>
+        <v>202</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>277</v>
+        <v>195</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E34" s="1" t="s">
-        <v>263</v>
+      <c r="E34" s="11" t="s">
+        <v>254</v>
       </c>
       <c r="F34" s="10" t="s">
         <v>27</v>
@@ -4350,7 +4344,7 @@
         <v>24</v>
       </c>
       <c r="I34" s="9" t="s">
-        <v>269</v>
+        <v>187</v>
       </c>
       <c r="J34" s="9"/>
       <c r="K34" s="9"/>
@@ -4362,19 +4356,19 @@
     </row>
     <row r="35" spans="1:16" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>285</v>
+        <v>203</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>277</v>
+        <v>195</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E35" s="1" t="s">
-        <v>264</v>
+      <c r="E35" s="11" t="s">
+        <v>255</v>
       </c>
       <c r="F35" s="10" t="s">
         <v>27</v>
@@ -4386,7 +4380,7 @@
         <v>24</v>
       </c>
       <c r="I35" s="9" t="s">
-        <v>269</v>
+        <v>187</v>
       </c>
       <c r="J35" s="9"/>
       <c r="K35" s="9"/>
@@ -4398,19 +4392,19 @@
     </row>
     <row r="36" spans="1:16" ht="135" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>286</v>
+        <v>204</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>277</v>
+        <v>195</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E36" s="1" t="s">
-        <v>265</v>
+      <c r="E36" s="11" t="s">
+        <v>256</v>
       </c>
       <c r="F36" s="10" t="s">
         <v>11</v>
@@ -4422,10 +4416,10 @@
         <v>25</v>
       </c>
       <c r="I36" s="9" t="s">
-        <v>269</v>
+        <v>187</v>
       </c>
       <c r="J36" s="9" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="K36" s="4" t="s">
         <v>33</v>
@@ -4438,25 +4432,25 @@
       </c>
       <c r="N36" s="9"/>
       <c r="O36" s="1" t="s">
-        <v>287</v>
+        <v>205</v>
       </c>
       <c r="P36" s="9"/>
     </row>
     <row r="37" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="B37" s="37" t="s">
-        <v>288</v>
+        <v>206</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>277</v>
+        <v>195</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E37" s="1" t="s">
-        <v>266</v>
+      <c r="E37" s="11" t="s">
+        <v>257</v>
       </c>
       <c r="F37" s="10" t="s">
         <v>27</v>
@@ -4468,7 +4462,7 @@
         <v>24</v>
       </c>
       <c r="I37" s="9" t="s">
-        <v>269</v>
+        <v>187</v>
       </c>
       <c r="J37" s="9"/>
       <c r="K37" s="9"/>
@@ -6223,7 +6217,7 @@
           <x14:formula1>
             <xm:f>Settings!$B$4:$B$6</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F8 F13:F22 F38:F158</xm:sqref>
+          <xm:sqref>F2:F8 F13:F23 F38:F158</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -6241,7 +6235,7 @@
           <x14:formula1>
             <xm:f>[1]Settings!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>F9:F12 F23 H9:H23</xm:sqref>
+          <xm:sqref>F9:F12 H9:H23</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -6280,8 +6274,8 @@
   </sheetPr>
   <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:B37"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6324,16 +6318,16 @@
     </row>
     <row r="2" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>74</v>
+        <v>306</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>72</v>
+        <v>258</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -6348,16 +6342,16 @@
     </row>
     <row r="3" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>89</v>
+        <v>307</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>93</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="2"/>
@@ -6371,16 +6365,16 @@
     </row>
     <row r="4" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>90</v>
+        <v>308</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>83</v>
+        <v>260</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -6394,16 +6388,16 @@
     </row>
     <row r="5" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>91</v>
+        <v>309</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>84</v>
+        <v>261</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -6417,16 +6411,16 @@
     </row>
     <row r="6" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>103</v>
+        <v>310</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>98</v>
+        <v>262</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -6440,16 +6434,16 @@
     </row>
     <row r="7" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>104</v>
+        <v>311</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>101</v>
+        <v>263</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -6463,16 +6457,16 @@
     </row>
     <row r="8" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>105</v>
+        <v>312</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>102</v>
+        <v>264</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -6486,16 +6480,16 @@
     </row>
     <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>114</v>
+        <v>313</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>110</v>
+        <v>265</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>115</v>
+        <v>93</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>116</v>
+        <v>94</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -6509,19 +6503,19 @@
     </row>
     <row r="10" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>194</v>
+        <v>314</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>161</v>
+        <v>266</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>195</v>
+        <v>138</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>196</v>
+        <v>139</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>197</v>
+        <v>140</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -6534,19 +6528,19 @@
     </row>
     <row r="11" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>198</v>
+        <v>315</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>165</v>
+        <v>267</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>199</v>
+        <v>141</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>200</v>
+        <v>142</v>
       </c>
       <c r="E11" s="33" t="s">
-        <v>201</v>
+        <v>143</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -6559,19 +6553,19 @@
     </row>
     <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>202</v>
+        <v>316</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>167</v>
+        <v>268</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>203</v>
+        <v>144</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>204</v>
+        <v>145</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>205</v>
+        <v>146</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -6584,19 +6578,19 @@
     </row>
     <row r="13" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>206</v>
+        <v>317</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>169</v>
+        <v>269</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>207</v>
+        <v>147</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>208</v>
+        <v>148</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>205</v>
+        <v>146</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -6609,19 +6603,19 @@
     </row>
     <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>171</v>
+        <v>270</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>210</v>
+        <v>149</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>211</v>
+        <v>150</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>205</v>
+        <v>146</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -6634,19 +6628,19 @@
     </row>
     <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>212</v>
+        <v>319</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>173</v>
+        <v>271</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>213</v>
+        <v>151</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>214</v>
+        <v>152</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>205</v>
+        <v>146</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -6659,19 +6653,19 @@
     </row>
     <row r="16" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>215</v>
+        <v>320</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>175</v>
+        <v>272</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>216</v>
+        <v>153</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>217</v>
+        <v>154</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>205</v>
+        <v>146</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -6684,19 +6678,19 @@
     </row>
     <row r="17" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>218</v>
+        <v>321</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>179</v>
+        <v>273</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>219</v>
+        <v>155</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>220</v>
+        <v>156</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>205</v>
+        <v>146</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -6709,19 +6703,19 @@
     </row>
     <row r="18" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>221</v>
+        <v>322</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>182</v>
+        <v>274</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>222</v>
+        <v>157</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>223</v>
+        <v>158</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>205</v>
+        <v>146</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -6734,19 +6728,19 @@
     </row>
     <row r="19" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>224</v>
+        <v>323</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>184</v>
+        <v>275</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>225</v>
+        <v>159</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>226</v>
+        <v>160</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>205</v>
+        <v>146</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -6759,266 +6753,266 @@
     </row>
     <row r="20" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>227</v>
+        <v>324</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>186</v>
+        <v>276</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>228</v>
+        <v>161</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>229</v>
+        <v>162</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>205</v>
+        <v>146</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>230</v>
+        <v>325</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>188</v>
+        <v>277</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>231</v>
+        <v>163</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>232</v>
+        <v>164</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>205</v>
+        <v>146</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>233</v>
+        <v>326</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>190</v>
+        <v>278</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>234</v>
+        <v>165</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>235</v>
+        <v>166</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>236</v>
+        <v>167</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>237</v>
+        <v>327</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>192</v>
+        <v>279</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>238</v>
+        <v>168</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>239</v>
+        <v>169</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>240</v>
+        <v>170</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>306</v>
+        <v>207</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>307</v>
+        <v>208</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>308</v>
+        <v>209</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>309</v>
+        <v>210</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>310</v>
+        <v>211</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>309</v>
+        <v>210</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>308</v>
+        <v>209</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>309</v>
+        <v>210</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>310</v>
+        <v>211</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>309</v>
+        <v>210</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>311</v>
+        <v>212</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>312</v>
+        <v>213</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>313</v>
+        <v>214</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>314</v>
+        <v>215</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>315</v>
+        <v>216</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>316</v>
+        <v>217</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>317</v>
+        <v>218</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>318</v>
+        <v>219</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>319</v>
+        <v>220</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>320</v>
+        <v>221</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>321</v>
+        <v>222</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>322</v>
+        <v>223</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>323</v>
+        <v>224</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>324</v>
+        <v>225</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>325</v>
+        <v>226</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>326</v>
+        <v>227</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>327</v>
+        <v>228</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>328</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -7227,18 +7221,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7258,18 +7252,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A346E62E-1A2C-4E03-B91F-FE4FC47F8E89}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEF49AB9-68C3-4E70-84F5-930D4AF0373D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A346E62E-1A2C-4E03-B91F-FE4FC47F8E89}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>